<commit_message>
Update xlsx forms and formDef.json to hide notes in contents screen.
</commit_message>
<xml_diff>
--- a/form-files/tables/breathcounter/forms/breathcounter/breathcounter.xlsx
+++ b/form-files/tables/breathcounter/forms/breathcounter/breathcounter.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2592" yWindow="624" windowWidth="11196" windowHeight="5244" activeTab="2"/>
+    <workbookView xWindow="2600" yWindow="620" windowWidth="21840" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="prompt_types" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>type</t>
   </si>
@@ -67,6 +72,9 @@
   </si>
   <si>
     <t>display.hint</t>
+  </si>
+  <si>
+    <t>hideInContents</t>
   </si>
 </sst>
 </file>
@@ -412,21 +420,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +448,11 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -456,6 +468,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -467,13 +484,13 @@
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -481,7 +498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -489,10 +506,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="1:2" ht="15" customHeight="1"/>
+    <row r="4" spans="1:2" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -500,18 +522,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -522,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -530,7 +552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -538,7 +560,7 @@
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -546,8 +568,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="5" spans="1:3" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>